<commit_message>
feat: update template & update officer
</commit_message>
<xml_diff>
--- a/agenda_generator/templates/ToastMaster_Template.xlsx
+++ b/agenda_generator/templates/ToastMaster_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\STCVM-L31\share_folder\toastmaster_agenda_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ms-toastmaster\agenda_generator\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A947FBB3-E84E-43F7-9A3B-F77BA03AFD9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCBE07F-FBDE-422A-9808-933926710667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda-1" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="363">
   <si>
     <t>Welcome to Microsoft Beijing Toastmasters Club</t>
   </si>
@@ -1161,6 +1161,9 @@
   </si>
   <si>
     <t>Prepared Speaker3</t>
+  </si>
+  <si>
+    <t>Conclusion &amp; Meeting Closing</t>
   </si>
 </sst>
 </file>
@@ -3301,6 +3304,102 @@
     <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="19" fillId="3" borderId="7" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="46" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="3" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="5" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="25" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="15" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="48" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3310,121 +3409,18 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="18" fontId="17" fillId="0" borderId="7" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="46" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="3" borderId="7" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="3" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="5" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="25" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="25" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="15" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="60" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="62" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="167" fontId="50" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3437,6 +3433,7 @@
     <xf numFmtId="167" fontId="50" fillId="0" borderId="5" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="60" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="61" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="61" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="61" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -3445,6 +3442,12 @@
     </xf>
     <xf numFmtId="167" fontId="50" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="52" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="62" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="349">
@@ -4162,8 +4165,8 @@
   </sheetPr>
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4185,108 +4188,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="195"/>
-      <c r="H1" s="196"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="189"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="191"/>
     </row>
     <row r="2" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="192" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="181"/>
-      <c r="C2" s="181"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="194"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="196"/>
+      <c r="B2" s="186"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="190"/>
+      <c r="H2" s="191"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="190"/>
-      <c r="E3" s="193"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="196"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="186"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="189"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="191"/>
       <c r="I3" s="35"/>
       <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A4" s="201" t="s">
+      <c r="A4" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="205"/>
-      <c r="D4" s="206"/>
-      <c r="E4" s="207"/>
-      <c r="F4" s="208"/>
-      <c r="G4" s="209"/>
-      <c r="H4" s="210"/>
+      <c r="C4" s="198"/>
+      <c r="D4" s="199"/>
+      <c r="E4" s="200"/>
+      <c r="F4" s="201"/>
+      <c r="G4" s="202"/>
+      <c r="H4" s="203"/>
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A5" s="202"/>
-      <c r="B5" s="205"/>
-      <c r="C5" s="205"/>
-      <c r="D5" s="206"/>
-      <c r="E5" s="207"/>
-      <c r="F5" s="208"/>
-      <c r="G5" s="209"/>
-      <c r="H5" s="210"/>
+      <c r="A5" s="195"/>
+      <c r="B5" s="198"/>
+      <c r="C5" s="198"/>
+      <c r="D5" s="199"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="201"/>
+      <c r="G5" s="202"/>
+      <c r="H5" s="203"/>
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" hidden="1" customHeight="1">
-      <c r="A6" s="202"/>
-      <c r="B6" s="205"/>
-      <c r="C6" s="205"/>
-      <c r="D6" s="206"/>
-      <c r="E6" s="207"/>
-      <c r="F6" s="208"/>
-      <c r="G6" s="209"/>
-      <c r="H6" s="210"/>
+      <c r="A6" s="195"/>
+      <c r="B6" s="198"/>
+      <c r="C6" s="198"/>
+      <c r="D6" s="199"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="201"/>
+      <c r="G6" s="202"/>
+      <c r="H6" s="203"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:12" ht="10.5" hidden="1" customHeight="1">
-      <c r="A7" s="203"/>
-      <c r="B7" s="211"/>
-      <c r="C7" s="211"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="214"/>
-      <c r="G7" s="215"/>
-      <c r="H7" s="216"/>
+      <c r="A7" s="196"/>
+      <c r="B7" s="204"/>
+      <c r="C7" s="204"/>
+      <c r="D7" s="205"/>
+      <c r="E7" s="206"/>
+      <c r="F7" s="207"/>
+      <c r="G7" s="208"/>
+      <c r="H7" s="209"/>
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A8" s="197" t="s">
+      <c r="A8" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="183"/>
-      <c r="C8" s="183"/>
-      <c r="D8" s="184"/>
-      <c r="E8" s="185"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="187"/>
-      <c r="H8" s="188"/>
+      <c r="B8" s="179"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="183"/>
+      <c r="H8" s="184"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
     </row>
@@ -4357,13 +4360,13 @@
         <v>1.791666666666667</v>
       </c>
       <c r="B11" s="73" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C11" s="69" t="s">
         <v>330</v>
       </c>
       <c r="D11" s="99" t="str">
-        <f>Roles!B3</f>
+        <f>Roles!B4</f>
         <v>Harper</v>
       </c>
       <c r="E11" s="76">
@@ -4384,7 +4387,7 @@
         <v>6.7944444444444452</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="24" customHeight="1">
+    <row r="12" spans="1:12" ht="23.25" customHeight="1">
       <c r="A12" s="20">
         <f t="shared" si="0"/>
         <v>6.7944444444444452</v>
@@ -4419,45 +4422,27 @@
         <v>6.7944444444444452</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="24" customHeight="1">
-      <c r="A13" s="20">
-        <f t="shared" si="0"/>
-        <v>6.7944444444444452</v>
-      </c>
-      <c r="B13" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="73" t="s">
-        <v>335</v>
-      </c>
-      <c r="D13" s="99" t="str">
-        <f>Roles!B4</f>
-        <v>Harper</v>
-      </c>
-      <c r="E13" s="76">
-        <v>5</v>
-      </c>
-      <c r="F13" s="151">
-        <v>3</v>
-      </c>
-      <c r="G13" s="152">
-        <v>4</v>
-      </c>
-      <c r="H13" s="153">
-        <v>5</v>
-      </c>
+    <row r="13" spans="1:12" ht="4.5" hidden="1" customHeight="1">
+      <c r="A13" s="20"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="151"/>
+      <c r="G13" s="152"/>
+      <c r="H13" s="153"/>
       <c r="I13" s="37">
-        <v>1.0034722222222201</v>
+        <v>1</v>
       </c>
       <c r="J13" s="36">
         <f t="shared" si="1"/>
-        <v>7.7979166666666657</v>
+        <v>7.7944444444444452</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="24" customHeight="1">
       <c r="A14" s="20">
         <f t="shared" si="0"/>
-        <v>7.7979166666666657</v>
+        <v>7.7944444444444452</v>
       </c>
       <c r="B14" s="73" t="s">
         <v>21</v>
@@ -4482,7 +4467,7 @@
       </c>
       <c r="J14" s="36">
         <f t="shared" si="1"/>
-        <v>7.7986111111111098</v>
+        <v>7.7951388888888893</v>
       </c>
       <c r="K14" s="36"/>
       <c r="L14" s="34"/>
@@ -4490,7 +4475,7 @@
     <row r="15" spans="1:12" ht="24.75" customHeight="1">
       <c r="A15" s="20">
         <f t="shared" si="0"/>
-        <v>7.7986111111111098</v>
+        <v>7.7951388888888893</v>
       </c>
       <c r="B15" s="73" t="s">
         <v>23</v>
@@ -4515,7 +4500,7 @@
       </c>
       <c r="J15" s="36">
         <f t="shared" si="1"/>
-        <v>8.7993055555555504</v>
+        <v>8.795833333333329</v>
       </c>
       <c r="K15" s="36"/>
       <c r="L15" s="34"/>
@@ -4523,7 +4508,7 @@
     <row r="16" spans="1:12" ht="24" customHeight="1">
       <c r="A16" s="20">
         <f t="shared" si="0"/>
-        <v>8.7993055555555504</v>
+        <v>8.795833333333329</v>
       </c>
       <c r="B16" s="73" t="s">
         <v>25</v>
@@ -4548,7 +4533,7 @@
       </c>
       <c r="J16" s="36">
         <f t="shared" si="1"/>
-        <v>8.7999999999999954</v>
+        <v>8.7965277777777739</v>
       </c>
       <c r="K16" s="36"/>
       <c r="L16" s="34"/>
@@ -4556,7 +4541,7 @@
     <row r="17" spans="1:12" ht="24" customHeight="1">
       <c r="A17" s="20">
         <f t="shared" si="0"/>
-        <v>8.7999999999999954</v>
+        <v>8.7965277777777739</v>
       </c>
       <c r="B17" s="73" t="s">
         <v>27</v>
@@ -4583,7 +4568,7 @@
       </c>
       <c r="J17" s="36">
         <f t="shared" si="1"/>
-        <v>8.8013888888888836</v>
+        <v>8.7979166666666622</v>
       </c>
       <c r="K17" s="36"/>
       <c r="L17" s="34"/>
@@ -4591,7 +4576,7 @@
     <row r="18" spans="1:12" ht="24" customHeight="1">
       <c r="A18" s="20">
         <f t="shared" si="0"/>
-        <v>8.8013888888888836</v>
+        <v>8.7979166666666622</v>
       </c>
       <c r="B18" s="73" t="s">
         <v>21</v>
@@ -4616,13 +4601,13 @@
       </c>
       <c r="J18" s="36">
         <f t="shared" si="1"/>
-        <v>8.8013888888888836</v>
+        <v>8.7979166666666622</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="24" customHeight="1" thickBot="1">
       <c r="A19" s="125">
         <f t="shared" si="0"/>
-        <v>8.8013888888888836</v>
+        <v>8.7979166666666622</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>20</v>
@@ -4647,32 +4632,32 @@
       </c>
       <c r="J19" s="36">
         <f t="shared" si="1"/>
-        <v>8.8020833333333286</v>
+        <v>8.7986111111111072</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A20" s="182" t="s">
+      <c r="A20" s="213" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="183"/>
-      <c r="C20" s="183"/>
-      <c r="D20" s="184"/>
-      <c r="E20" s="185"/>
-      <c r="F20" s="186"/>
-      <c r="G20" s="187"/>
-      <c r="H20" s="188"/>
+      <c r="B20" s="179"/>
+      <c r="C20" s="179"/>
+      <c r="D20" s="180"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="183"/>
+      <c r="H20" s="184"/>
       <c r="I20" s="37">
         <v>0</v>
       </c>
       <c r="J20" s="36">
         <f t="shared" si="1"/>
-        <v>8.8020833333333286</v>
+        <v>8.7986111111111072</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="24" customHeight="1">
       <c r="A21" s="20">
         <f>J20</f>
-        <v>8.8020833333333286</v>
+        <v>8.7986111111111072</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>31</v>
@@ -4701,13 +4686,13 @@
       </c>
       <c r="J21" s="36">
         <f t="shared" si="1"/>
-        <v>8.8159722222222179</v>
+        <v>8.8124999999999964</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="24" customHeight="1">
       <c r="A22" s="20">
         <f>J21</f>
-        <v>8.8159722222222179</v>
+        <v>8.8124999999999964</v>
       </c>
       <c r="B22" s="70" t="s">
         <v>32</v>
@@ -4736,13 +4721,13 @@
       </c>
       <c r="J22" s="36">
         <f t="shared" si="1"/>
-        <v>8.8201388888888843</v>
+        <v>8.8166666666666629</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="24" customHeight="1">
       <c r="A23" s="20">
         <f>J22</f>
-        <v>8.8201388888888843</v>
+        <v>8.8166666666666629</v>
       </c>
       <c r="B23" s="70" t="s">
         <v>20</v>
@@ -4769,13 +4754,13 @@
       </c>
       <c r="J23" s="36">
         <f t="shared" si="1"/>
-        <v>8.8208333333333293</v>
+        <v>8.8173611111111079</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="24" customHeight="1" thickBot="1">
       <c r="A24" s="129">
         <f>J23</f>
-        <v>8.8208333333333293</v>
+        <v>8.8173611111111079</v>
       </c>
       <c r="B24" s="130" t="s">
         <v>36</v>
@@ -4798,26 +4783,26 @@
       </c>
       <c r="J24" s="36">
         <f t="shared" si="1"/>
-        <v>8.8256944444444407</v>
+        <v>8.8222222222222193</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A25" s="182" t="s">
+      <c r="A25" s="213" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="183"/>
-      <c r="C25" s="183"/>
-      <c r="D25" s="184"/>
-      <c r="E25" s="185"/>
-      <c r="F25" s="186"/>
-      <c r="G25" s="187"/>
-      <c r="H25" s="188"/>
+      <c r="B25" s="179"/>
+      <c r="C25" s="179"/>
+      <c r="D25" s="180"/>
+      <c r="E25" s="181"/>
+      <c r="F25" s="182"/>
+      <c r="G25" s="183"/>
+      <c r="H25" s="184"/>
       <c r="I25" s="37">
         <v>1</v>
       </c>
       <c r="J25" s="36">
         <f t="shared" si="1"/>
-        <v>9.8256944444444407</v>
+        <v>9.8222222222222193</v>
       </c>
       <c r="K25" s="36"/>
       <c r="L25" s="34"/>
@@ -4825,7 +4810,7 @@
     <row r="26" spans="1:12" ht="24" customHeight="1">
       <c r="A26" s="20">
         <f t="shared" ref="A26:A27" si="2">J25</f>
-        <v>9.8256944444444407</v>
+        <v>9.8222222222222193</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>20</v>
@@ -4852,7 +4837,7 @@
       </c>
       <c r="J26" s="36">
         <f t="shared" si="1"/>
-        <v>9.8263888888888857</v>
+        <v>9.8229166666666643</v>
       </c>
       <c r="K26" s="36"/>
       <c r="L26" s="34"/>
@@ -4860,7 +4845,7 @@
     <row r="27" spans="1:12" ht="47.25" customHeight="1" thickBot="1">
       <c r="A27" s="20">
         <f t="shared" si="2"/>
-        <v>9.8263888888888857</v>
+        <v>9.8229166666666643</v>
       </c>
       <c r="B27" s="73" t="s">
         <v>39</v>
@@ -4889,26 +4874,26 @@
       </c>
       <c r="J27" s="36">
         <f t="shared" si="1"/>
-        <v>9.8312499999999972</v>
+        <v>9.8277777777777757</v>
       </c>
       <c r="K27" s="36"/>
       <c r="L27" s="34"/>
     </row>
     <row r="28" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A28" s="182" t="s">
+      <c r="A28" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="183"/>
-      <c r="C28" s="183"/>
-      <c r="D28" s="184"/>
-      <c r="E28" s="185"/>
-      <c r="F28" s="186"/>
-      <c r="G28" s="187"/>
-      <c r="H28" s="188"/>
+      <c r="B28" s="179"/>
+      <c r="C28" s="179"/>
+      <c r="D28" s="180"/>
+      <c r="E28" s="181"/>
+      <c r="F28" s="182"/>
+      <c r="G28" s="183"/>
+      <c r="H28" s="184"/>
       <c r="I28" s="37"/>
       <c r="J28" s="36">
         <f>J27+I28</f>
-        <v>9.8312499999999972</v>
+        <v>9.8277777777777757</v>
       </c>
       <c r="K28" s="36"/>
       <c r="L28" s="34"/>
@@ -4916,7 +4901,7 @@
     <row r="29" spans="1:12" ht="24" customHeight="1">
       <c r="A29" s="20">
         <f>J28</f>
-        <v>9.8312499999999972</v>
+        <v>9.8277777777777757</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>21</v>
@@ -4943,7 +4928,7 @@
       </c>
       <c r="J29" s="36">
         <f t="shared" si="1"/>
-        <v>10.831944444444437</v>
+        <v>10.828472222222215</v>
       </c>
       <c r="K29" s="36"/>
       <c r="L29" s="34"/>
@@ -4951,7 +4936,7 @@
     <row r="30" spans="1:12" ht="24" customHeight="1">
       <c r="A30" s="20">
         <f>J29</f>
-        <v>10.831944444444437</v>
+        <v>10.828472222222215</v>
       </c>
       <c r="B30" s="55" t="s">
         <v>338</v>
@@ -4980,7 +4965,7 @@
       </c>
       <c r="J30" s="36">
         <f t="shared" si="1"/>
-        <v>10.83402777777777</v>
+        <v>10.830555555555549</v>
       </c>
       <c r="K30" s="36"/>
       <c r="L30" s="34"/>
@@ -4988,7 +4973,7 @@
     <row r="31" spans="1:12" ht="24" customHeight="1">
       <c r="A31" s="20">
         <f>J30</f>
-        <v>10.83402777777777</v>
+        <v>10.830555555555549</v>
       </c>
       <c r="B31" s="55" t="s">
         <v>25</v>
@@ -5015,7 +5000,7 @@
       </c>
       <c r="J31" s="36">
         <f>J30+I31</f>
-        <v>10.835416666666658</v>
+        <v>10.831944444444437</v>
       </c>
       <c r="K31" s="36"/>
       <c r="L31" s="38"/>
@@ -5023,7 +5008,7 @@
     <row r="32" spans="1:12" ht="24" customHeight="1">
       <c r="A32" s="20">
         <f t="shared" ref="A32:A35" si="3">J31</f>
-        <v>10.835416666666658</v>
+        <v>10.831944444444437</v>
       </c>
       <c r="B32" s="55" t="s">
         <v>27</v>
@@ -5052,7 +5037,7 @@
       </c>
       <c r="J32" s="36">
         <f t="shared" si="1"/>
-        <v>10.837499999999991</v>
+        <v>10.83402777777777</v>
       </c>
       <c r="K32" s="36"/>
       <c r="L32" s="38"/>
@@ -5060,7 +5045,7 @@
     <row r="33" spans="1:12" ht="24" customHeight="1">
       <c r="A33" s="20">
         <f t="shared" si="3"/>
-        <v>10.837499999999991</v>
+        <v>10.83402777777777</v>
       </c>
       <c r="B33" s="55" t="s">
         <v>23</v>
@@ -5087,40 +5072,26 @@
       </c>
       <c r="J33" s="36">
         <f t="shared" si="1"/>
-        <v>10.83888888888888</v>
+        <v>10.835416666666658</v>
       </c>
       <c r="K33" s="36"/>
       <c r="L33" s="38"/>
     </row>
-    <row r="34" spans="1:12" ht="24" customHeight="1">
-      <c r="A34" s="20">
-        <f t="shared" si="3"/>
-        <v>10.83888888888888</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="157" t="s">
-        <v>340</v>
-      </c>
-      <c r="D34" s="99" t="str">
-        <f>Roles!B2</f>
-        <v>Davie</v>
-      </c>
-      <c r="E34" s="76">
-        <v>1</v>
-      </c>
+    <row r="34" spans="1:12" ht="1.5" customHeight="1">
+      <c r="A34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="157"/>
+      <c r="D34" s="99"/>
+      <c r="E34" s="76"/>
       <c r="F34" s="151"/>
       <c r="G34" s="152"/>
-      <c r="H34" s="153">
-        <v>1</v>
-      </c>
+      <c r="H34" s="153"/>
       <c r="I34" s="37">
-        <v>6.9444444444444404E-4</v>
+        <v>0</v>
       </c>
       <c r="J34" s="36">
         <f t="shared" si="1"/>
-        <v>10.839583333333325</v>
+        <v>10.835416666666658</v>
       </c>
       <c r="K34" s="36"/>
       <c r="L34" s="38"/>
@@ -5128,7 +5099,7 @@
     <row r="35" spans="1:12" ht="24" customHeight="1">
       <c r="A35" s="20">
         <f t="shared" si="3"/>
-        <v>10.839583333333325</v>
+        <v>10.835416666666658</v>
       </c>
       <c r="B35" s="73" t="s">
         <v>21</v>
@@ -5157,7 +5128,7 @@
       </c>
       <c r="J35" s="36">
         <f t="shared" si="1"/>
-        <v>11.843055555555548</v>
+        <v>11.838888888888881</v>
       </c>
       <c r="K35" s="36"/>
       <c r="L35" s="38"/>
@@ -5165,13 +5136,13 @@
     <row r="36" spans="1:12" ht="24" customHeight="1" thickBot="1">
       <c r="A36" s="77">
         <f>J35</f>
-        <v>11.843055555555548</v>
+        <v>11.838888888888881</v>
       </c>
       <c r="B36" s="70" t="s">
         <v>20</v>
       </c>
       <c r="C36" s="73" t="s">
-        <v>344</v>
+        <v>362</v>
       </c>
       <c r="D36" s="99" t="str">
         <f>Roles!B4</f>
@@ -5194,49 +5165,30 @@
       </c>
       <c r="J36" s="36">
         <f>J35+I36</f>
-        <v>12.844444444444438</v>
+        <v>12.840277777777771</v>
       </c>
       <c r="K36" s="36"/>
       <c r="L36" s="38"/>
     </row>
-    <row r="37" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A37" s="77">
-        <f>J36</f>
-        <v>12.844444444444438</v>
-      </c>
-      <c r="B37" s="78" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="122" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" s="99" t="str">
-        <f>Roles!B3</f>
-        <v>Harper</v>
-      </c>
-      <c r="E37" s="71">
-        <v>2</v>
-      </c>
+    <row r="37" spans="1:12" ht="1.5" customHeight="1" thickBot="1">
+      <c r="A37" s="77"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="122"/>
+      <c r="D37" s="99"/>
+      <c r="E37" s="71"/>
       <c r="F37" s="109"/>
       <c r="G37" s="110"/>
-      <c r="H37" s="111" t="s">
-        <v>56</v>
-      </c>
-      <c r="I37" s="37">
-        <v>1.0013888888888889</v>
-      </c>
-      <c r="J37" s="36">
-        <f>J35+I37</f>
-        <v>12.844444444444436</v>
-      </c>
+      <c r="H37" s="111"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="36"/>
       <c r="K37" s="39"/>
       <c r="L37" s="12"/>
     </row>
     <row r="38" spans="1:12" ht="21" customHeight="1">
-      <c r="A38" s="189"/>
-      <c r="B38" s="181"/>
-      <c r="C38" s="181"/>
-      <c r="D38" s="190"/>
+      <c r="A38" s="214"/>
+      <c r="B38" s="186"/>
+      <c r="C38" s="186"/>
+      <c r="D38" s="187"/>
       <c r="E38" s="12"/>
       <c r="F38" s="43"/>
       <c r="G38" s="44"/>
@@ -5247,37 +5199,37 @@
       <c r="L38" s="12"/>
     </row>
     <row r="39" spans="1:12" ht="101.25" customHeight="1">
-      <c r="A39" s="191" t="s">
+      <c r="A39" s="215" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="181"/>
-      <c r="C39" s="181"/>
-      <c r="D39" s="192"/>
-      <c r="E39" s="193"/>
-      <c r="F39" s="194"/>
-      <c r="G39" s="195"/>
-      <c r="H39" s="196"/>
+      <c r="B39" s="186"/>
+      <c r="C39" s="186"/>
+      <c r="D39" s="216"/>
+      <c r="E39" s="188"/>
+      <c r="F39" s="189"/>
+      <c r="G39" s="190"/>
+      <c r="H39" s="191"/>
       <c r="I39" s="39"/>
       <c r="J39" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K39" s="178"/>
+      <c r="K39" s="210"/>
       <c r="L39" s="12"/>
     </row>
     <row r="40" spans="1:12" ht="145.5" customHeight="1">
-      <c r="A40" s="180" t="s">
+      <c r="A40" s="212" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="181"/>
-      <c r="C40" s="181"/>
-      <c r="D40" s="190"/>
-      <c r="E40" s="193"/>
-      <c r="F40" s="194"/>
-      <c r="G40" s="195"/>
-      <c r="H40" s="196"/>
+      <c r="B40" s="186"/>
+      <c r="C40" s="186"/>
+      <c r="D40" s="187"/>
+      <c r="E40" s="188"/>
+      <c r="F40" s="189"/>
+      <c r="G40" s="190"/>
+      <c r="H40" s="191"/>
       <c r="I40" s="39"/>
       <c r="J40" s="52"/>
-      <c r="K40" s="179"/>
+      <c r="K40" s="211"/>
     </row>
     <row r="41" spans="1:12" ht="12.75" customHeight="1">
       <c r="A41" s="28"/>
@@ -5618,12 +5570,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:H7"/>
     <mergeCell ref="K39:K40"/>
     <mergeCell ref="A40:C40"/>
     <mergeCell ref="A20:H20"/>
@@ -5632,6 +5578,12 @@
     <mergeCell ref="A38:D38"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="D39:H40"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:H7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5669,108 +5621,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="195"/>
-      <c r="H1" s="196"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="189"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="191"/>
     </row>
     <row r="2" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="192" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="181"/>
-      <c r="C2" s="181"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="194"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="196"/>
+      <c r="B2" s="186"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="190"/>
+      <c r="H2" s="191"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="190"/>
-      <c r="E3" s="193"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="196"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="186"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="189"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="191"/>
       <c r="I3" s="35"/>
       <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A4" s="201" t="s">
+      <c r="A4" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="205"/>
-      <c r="D4" s="206"/>
-      <c r="E4" s="207"/>
-      <c r="F4" s="208"/>
-      <c r="G4" s="209"/>
-      <c r="H4" s="210"/>
+      <c r="C4" s="198"/>
+      <c r="D4" s="199"/>
+      <c r="E4" s="200"/>
+      <c r="F4" s="201"/>
+      <c r="G4" s="202"/>
+      <c r="H4" s="203"/>
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A5" s="202"/>
-      <c r="B5" s="205"/>
-      <c r="C5" s="205"/>
-      <c r="D5" s="206"/>
-      <c r="E5" s="207"/>
-      <c r="F5" s="208"/>
-      <c r="G5" s="209"/>
-      <c r="H5" s="210"/>
+      <c r="A5" s="195"/>
+      <c r="B5" s="198"/>
+      <c r="C5" s="198"/>
+      <c r="D5" s="199"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="201"/>
+      <c r="G5" s="202"/>
+      <c r="H5" s="203"/>
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" hidden="1" customHeight="1">
-      <c r="A6" s="202"/>
-      <c r="B6" s="205"/>
-      <c r="C6" s="205"/>
-      <c r="D6" s="206"/>
-      <c r="E6" s="207"/>
-      <c r="F6" s="208"/>
-      <c r="G6" s="209"/>
-      <c r="H6" s="210"/>
+      <c r="A6" s="195"/>
+      <c r="B6" s="198"/>
+      <c r="C6" s="198"/>
+      <c r="D6" s="199"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="201"/>
+      <c r="G6" s="202"/>
+      <c r="H6" s="203"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:12" ht="10.5" hidden="1" customHeight="1">
-      <c r="A7" s="203"/>
-      <c r="B7" s="211"/>
-      <c r="C7" s="211"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="214"/>
-      <c r="G7" s="215"/>
-      <c r="H7" s="216"/>
+      <c r="A7" s="196"/>
+      <c r="B7" s="204"/>
+      <c r="C7" s="204"/>
+      <c r="D7" s="205"/>
+      <c r="E7" s="206"/>
+      <c r="F7" s="207"/>
+      <c r="G7" s="208"/>
+      <c r="H7" s="209"/>
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A8" s="197" t="s">
+      <c r="A8" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="183"/>
-      <c r="C8" s="183"/>
-      <c r="D8" s="184"/>
-      <c r="E8" s="185"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="187"/>
-      <c r="H8" s="188"/>
+      <c r="B8" s="179"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="183"/>
+      <c r="H8" s="184"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
     </row>
@@ -6135,16 +6087,16 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A20" s="182" t="s">
+      <c r="A20" s="213" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="183"/>
-      <c r="C20" s="183"/>
-      <c r="D20" s="184"/>
-      <c r="E20" s="185"/>
-      <c r="F20" s="186"/>
-      <c r="G20" s="187"/>
-      <c r="H20" s="188"/>
+      <c r="B20" s="179"/>
+      <c r="C20" s="179"/>
+      <c r="D20" s="180"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="183"/>
+      <c r="H20" s="184"/>
       <c r="I20" s="37">
         <v>0</v>
       </c>
@@ -6286,16 +6238,16 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A25" s="182" t="s">
+      <c r="A25" s="213" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="183"/>
-      <c r="C25" s="183"/>
-      <c r="D25" s="184"/>
-      <c r="E25" s="185"/>
-      <c r="F25" s="186"/>
-      <c r="G25" s="187"/>
-      <c r="H25" s="188"/>
+      <c r="B25" s="179"/>
+      <c r="C25" s="179"/>
+      <c r="D25" s="180"/>
+      <c r="E25" s="181"/>
+      <c r="F25" s="182"/>
+      <c r="G25" s="183"/>
+      <c r="H25" s="184"/>
       <c r="I25" s="37">
         <v>1</v>
       </c>
@@ -6451,16 +6403,16 @@
       <c r="L29" s="34"/>
     </row>
     <row r="30" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A30" s="182" t="s">
+      <c r="A30" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="183"/>
-      <c r="C30" s="183"/>
-      <c r="D30" s="184"/>
-      <c r="E30" s="185"/>
-      <c r="F30" s="186"/>
-      <c r="G30" s="187"/>
-      <c r="H30" s="188"/>
+      <c r="B30" s="179"/>
+      <c r="C30" s="179"/>
+      <c r="D30" s="180"/>
+      <c r="E30" s="181"/>
+      <c r="F30" s="182"/>
+      <c r="G30" s="183"/>
+      <c r="H30" s="184"/>
       <c r="I30" s="37"/>
       <c r="J30" s="36">
         <f>J29+I30</f>
@@ -6826,10 +6778,10 @@
       <c r="L40" s="12"/>
     </row>
     <row r="41" spans="1:12" ht="21" customHeight="1">
-      <c r="A41" s="189"/>
-      <c r="B41" s="181"/>
-      <c r="C41" s="181"/>
-      <c r="D41" s="190"/>
+      <c r="A41" s="214"/>
+      <c r="B41" s="186"/>
+      <c r="C41" s="186"/>
+      <c r="D41" s="187"/>
       <c r="E41" s="12"/>
       <c r="F41" s="43"/>
       <c r="G41" s="44"/>
@@ -6840,37 +6792,37 @@
       <c r="L41" s="12"/>
     </row>
     <row r="42" spans="1:12" ht="101.25" customHeight="1">
-      <c r="A42" s="191" t="s">
+      <c r="A42" s="215" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="181"/>
-      <c r="C42" s="181"/>
-      <c r="D42" s="192"/>
-      <c r="E42" s="193"/>
-      <c r="F42" s="194"/>
-      <c r="G42" s="195"/>
-      <c r="H42" s="196"/>
+      <c r="B42" s="186"/>
+      <c r="C42" s="186"/>
+      <c r="D42" s="216"/>
+      <c r="E42" s="188"/>
+      <c r="F42" s="189"/>
+      <c r="G42" s="190"/>
+      <c r="H42" s="191"/>
       <c r="I42" s="39"/>
       <c r="J42" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K42" s="178"/>
+      <c r="K42" s="210"/>
       <c r="L42" s="12"/>
     </row>
     <row r="43" spans="1:12" ht="145.5" customHeight="1">
-      <c r="A43" s="180" t="s">
+      <c r="A43" s="212" t="s">
         <v>64</v>
       </c>
-      <c r="B43" s="181"/>
-      <c r="C43" s="181"/>
-      <c r="D43" s="190"/>
-      <c r="E43" s="193"/>
-      <c r="F43" s="194"/>
-      <c r="G43" s="195"/>
-      <c r="H43" s="196"/>
+      <c r="B43" s="186"/>
+      <c r="C43" s="186"/>
+      <c r="D43" s="187"/>
+      <c r="E43" s="188"/>
+      <c r="F43" s="189"/>
+      <c r="G43" s="190"/>
+      <c r="H43" s="191"/>
       <c r="I43" s="39"/>
       <c r="J43" s="52"/>
-      <c r="K43" s="179"/>
+      <c r="K43" s="211"/>
     </row>
     <row r="44" spans="1:12" ht="12.75" customHeight="1">
       <c r="A44" s="28"/>
@@ -7211,12 +7163,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:H7"/>
     <mergeCell ref="K42:K43"/>
     <mergeCell ref="A43:C43"/>
     <mergeCell ref="A20:H20"/>
@@ -7225,6 +7171,12 @@
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="D42:H43"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:H7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7239,7 +7191,7 @@
   </sheetPr>
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -7262,108 +7214,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="195"/>
-      <c r="H1" s="196"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="189"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="191"/>
     </row>
     <row r="2" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="192" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="181"/>
-      <c r="C2" s="181"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="194"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="196"/>
+      <c r="B2" s="186"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="190"/>
+      <c r="H2" s="191"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="193" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="190"/>
-      <c r="E3" s="193"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="196"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="186"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="189"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="191"/>
       <c r="I3" s="35"/>
       <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A4" s="201" t="s">
+      <c r="A4" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="205"/>
-      <c r="D4" s="206"/>
-      <c r="E4" s="207"/>
-      <c r="F4" s="208"/>
-      <c r="G4" s="209"/>
-      <c r="H4" s="210"/>
+      <c r="C4" s="198"/>
+      <c r="D4" s="199"/>
+      <c r="E4" s="200"/>
+      <c r="F4" s="201"/>
+      <c r="G4" s="202"/>
+      <c r="H4" s="203"/>
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A5" s="202"/>
-      <c r="B5" s="205"/>
-      <c r="C5" s="205"/>
-      <c r="D5" s="206"/>
-      <c r="E5" s="207"/>
-      <c r="F5" s="208"/>
-      <c r="G5" s="209"/>
-      <c r="H5" s="210"/>
+      <c r="A5" s="195"/>
+      <c r="B5" s="198"/>
+      <c r="C5" s="198"/>
+      <c r="D5" s="199"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="201"/>
+      <c r="G5" s="202"/>
+      <c r="H5" s="203"/>
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" hidden="1" customHeight="1">
-      <c r="A6" s="202"/>
-      <c r="B6" s="205"/>
-      <c r="C6" s="205"/>
-      <c r="D6" s="206"/>
-      <c r="E6" s="207"/>
-      <c r="F6" s="208"/>
-      <c r="G6" s="209"/>
-      <c r="H6" s="210"/>
+      <c r="A6" s="195"/>
+      <c r="B6" s="198"/>
+      <c r="C6" s="198"/>
+      <c r="D6" s="199"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="201"/>
+      <c r="G6" s="202"/>
+      <c r="H6" s="203"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:12" ht="10.5" hidden="1" customHeight="1">
-      <c r="A7" s="203"/>
-      <c r="B7" s="211"/>
-      <c r="C7" s="211"/>
-      <c r="D7" s="212"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="214"/>
-      <c r="G7" s="215"/>
-      <c r="H7" s="216"/>
+      <c r="A7" s="196"/>
+      <c r="B7" s="204"/>
+      <c r="C7" s="204"/>
+      <c r="D7" s="205"/>
+      <c r="E7" s="206"/>
+      <c r="F7" s="207"/>
+      <c r="G7" s="208"/>
+      <c r="H7" s="209"/>
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A8" s="197" t="s">
+      <c r="A8" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="183"/>
-      <c r="C8" s="183"/>
-      <c r="D8" s="184"/>
-      <c r="E8" s="185"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="187"/>
-      <c r="H8" s="188"/>
+      <c r="B8" s="179"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="183"/>
+      <c r="H8" s="184"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
     </row>
@@ -7728,16 +7680,16 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A20" s="182" t="s">
+      <c r="A20" s="213" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="183"/>
-      <c r="C20" s="183"/>
-      <c r="D20" s="184"/>
-      <c r="E20" s="185"/>
-      <c r="F20" s="186"/>
-      <c r="G20" s="187"/>
-      <c r="H20" s="188"/>
+      <c r="B20" s="179"/>
+      <c r="C20" s="179"/>
+      <c r="D20" s="180"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="183"/>
+      <c r="H20" s="184"/>
       <c r="I20" s="37">
         <v>0</v>
       </c>
@@ -7879,16 +7831,16 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A25" s="182" t="s">
+      <c r="A25" s="213" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="183"/>
-      <c r="C25" s="183"/>
-      <c r="D25" s="184"/>
-      <c r="E25" s="185"/>
-      <c r="F25" s="186"/>
-      <c r="G25" s="187"/>
-      <c r="H25" s="188"/>
+      <c r="B25" s="179"/>
+      <c r="C25" s="179"/>
+      <c r="D25" s="180"/>
+      <c r="E25" s="181"/>
+      <c r="F25" s="182"/>
+      <c r="G25" s="183"/>
+      <c r="H25" s="184"/>
       <c r="I25" s="37">
         <v>1</v>
       </c>
@@ -8116,16 +8068,16 @@
       <c r="L31" s="34"/>
     </row>
     <row r="32" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A32" s="182" t="s">
+      <c r="A32" s="213" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="183"/>
-      <c r="C32" s="183"/>
-      <c r="D32" s="184"/>
-      <c r="E32" s="185"/>
-      <c r="F32" s="186"/>
-      <c r="G32" s="187"/>
-      <c r="H32" s="188"/>
+      <c r="B32" s="179"/>
+      <c r="C32" s="179"/>
+      <c r="D32" s="180"/>
+      <c r="E32" s="181"/>
+      <c r="F32" s="182"/>
+      <c r="G32" s="183"/>
+      <c r="H32" s="184"/>
       <c r="I32" s="37"/>
       <c r="J32" s="36">
         <f>J31+I32</f>
@@ -8528,10 +8480,10 @@
       <c r="L43" s="12"/>
     </row>
     <row r="44" spans="1:12" ht="21" customHeight="1">
-      <c r="A44" s="189"/>
-      <c r="B44" s="181"/>
-      <c r="C44" s="181"/>
-      <c r="D44" s="190"/>
+      <c r="A44" s="214"/>
+      <c r="B44" s="186"/>
+      <c r="C44" s="186"/>
+      <c r="D44" s="187"/>
       <c r="E44" s="12"/>
       <c r="F44" s="43"/>
       <c r="G44" s="44"/>
@@ -8542,37 +8494,37 @@
       <c r="L44" s="12"/>
     </row>
     <row r="45" spans="1:12" ht="101.25" customHeight="1">
-      <c r="A45" s="191" t="s">
+      <c r="A45" s="215" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="181"/>
-      <c r="C45" s="181"/>
-      <c r="D45" s="192"/>
-      <c r="E45" s="193"/>
-      <c r="F45" s="194"/>
-      <c r="G45" s="195"/>
-      <c r="H45" s="196"/>
+      <c r="B45" s="186"/>
+      <c r="C45" s="186"/>
+      <c r="D45" s="216"/>
+      <c r="E45" s="188"/>
+      <c r="F45" s="189"/>
+      <c r="G45" s="190"/>
+      <c r="H45" s="191"/>
       <c r="I45" s="39"/>
       <c r="J45" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K45" s="178"/>
+      <c r="K45" s="210"/>
       <c r="L45" s="12"/>
     </row>
     <row r="46" spans="1:12" ht="145.5" customHeight="1">
-      <c r="A46" s="180" t="s">
+      <c r="A46" s="212" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="181"/>
-      <c r="C46" s="181"/>
-      <c r="D46" s="190"/>
-      <c r="E46" s="193"/>
-      <c r="F46" s="194"/>
-      <c r="G46" s="195"/>
-      <c r="H46" s="196"/>
+      <c r="B46" s="186"/>
+      <c r="C46" s="186"/>
+      <c r="D46" s="187"/>
+      <c r="E46" s="188"/>
+      <c r="F46" s="189"/>
+      <c r="G46" s="190"/>
+      <c r="H46" s="191"/>
       <c r="I46" s="39"/>
       <c r="J46" s="52"/>
-      <c r="K46" s="179"/>
+      <c r="K46" s="211"/>
     </row>
     <row r="47" spans="1:12" ht="12.75" customHeight="1">
       <c r="A47" s="28"/>
@@ -8913,6 +8865,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:H7"/>
     <mergeCell ref="K45:K46"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A20:H20"/>
@@ -8921,12 +8879,6 @@
     <mergeCell ref="A44:D44"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="D45:H46"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:H7"/>
-    <mergeCell ref="A8:H8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8964,112 +8916,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="185" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="195"/>
-      <c r="H1" s="196"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="189"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="191"/>
     </row>
     <row r="2" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A2" s="223" t="s">
+      <c r="A2" s="220" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="225"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="226"/>
-      <c r="H2" s="227"/>
+      <c r="B2" s="221"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="224"/>
+      <c r="H2" s="225"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A3" s="228" t="s">
+      <c r="A3" s="226" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="218"/>
-      <c r="C3" s="218"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="225"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="226"/>
-      <c r="H3" s="227"/>
+      <c r="B3" s="221"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="222"/>
+      <c r="E3" s="223"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="224"/>
+      <c r="H3" s="225"/>
       <c r="I3" s="35"/>
       <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A4" s="220" t="s">
+      <c r="A4" s="217" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="222" t="s">
+      <c r="B4" s="219" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="221"/>
-      <c r="D4" s="221"/>
-      <c r="E4" s="221"/>
-      <c r="F4" s="221"/>
-      <c r="G4" s="221"/>
-      <c r="H4" s="221"/>
+      <c r="C4" s="218"/>
+      <c r="D4" s="218"/>
+      <c r="E4" s="218"/>
+      <c r="F4" s="218"/>
+      <c r="G4" s="218"/>
+      <c r="H4" s="218"/>
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A5" s="221"/>
-      <c r="B5" s="221"/>
-      <c r="C5" s="221"/>
-      <c r="D5" s="221"/>
-      <c r="E5" s="221"/>
-      <c r="F5" s="221"/>
-      <c r="G5" s="221"/>
-      <c r="H5" s="221"/>
+      <c r="A5" s="218"/>
+      <c r="B5" s="218"/>
+      <c r="C5" s="218"/>
+      <c r="D5" s="218"/>
+      <c r="E5" s="218"/>
+      <c r="F5" s="218"/>
+      <c r="G5" s="218"/>
+      <c r="H5" s="218"/>
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" hidden="1" customHeight="1">
-      <c r="A6" s="220" t="s">
+      <c r="A6" s="217" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="222" t="s">
+      <c r="B6" s="219" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="221"/>
-      <c r="D6" s="221"/>
-      <c r="E6" s="221"/>
-      <c r="F6" s="221"/>
-      <c r="G6" s="221"/>
-      <c r="H6" s="221"/>
+      <c r="C6" s="218"/>
+      <c r="D6" s="218"/>
+      <c r="E6" s="218"/>
+      <c r="F6" s="218"/>
+      <c r="G6" s="218"/>
+      <c r="H6" s="218"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:12" ht="10.5" hidden="1" customHeight="1">
-      <c r="A7" s="221"/>
-      <c r="B7" s="221"/>
-      <c r="C7" s="221"/>
-      <c r="D7" s="221"/>
-      <c r="E7" s="221"/>
-      <c r="F7" s="221"/>
-      <c r="G7" s="221"/>
-      <c r="H7" s="221"/>
+      <c r="A7" s="218"/>
+      <c r="B7" s="218"/>
+      <c r="C7" s="218"/>
+      <c r="D7" s="218"/>
+      <c r="E7" s="218"/>
+      <c r="F7" s="218"/>
+      <c r="G7" s="218"/>
+      <c r="H7" s="218"/>
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A8" s="197" t="s">
+      <c r="A8" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="183"/>
-      <c r="C8" s="183"/>
-      <c r="D8" s="184"/>
-      <c r="E8" s="185"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="187"/>
-      <c r="H8" s="188"/>
+      <c r="B8" s="179"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="183"/>
+      <c r="H8" s="184"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
     </row>
@@ -9434,16 +9386,16 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A20" s="182" t="s">
+      <c r="A20" s="213" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="183"/>
-      <c r="C20" s="183"/>
-      <c r="D20" s="184"/>
-      <c r="E20" s="185"/>
-      <c r="F20" s="186"/>
-      <c r="G20" s="187"/>
-      <c r="H20" s="188"/>
+      <c r="B20" s="179"/>
+      <c r="C20" s="179"/>
+      <c r="D20" s="180"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="183"/>
+      <c r="H20" s="184"/>
       <c r="I20" s="37">
         <v>0</v>
       </c>
@@ -9587,16 +9539,16 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A25" s="182" t="s">
+      <c r="A25" s="213" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="183"/>
-      <c r="C25" s="183"/>
-      <c r="D25" s="184"/>
-      <c r="E25" s="185"/>
-      <c r="F25" s="186"/>
-      <c r="G25" s="187"/>
-      <c r="H25" s="188"/>
+      <c r="B25" s="179"/>
+      <c r="C25" s="179"/>
+      <c r="D25" s="180"/>
+      <c r="E25" s="181"/>
+      <c r="F25" s="182"/>
+      <c r="G25" s="183"/>
+      <c r="H25" s="184"/>
       <c r="I25" s="37">
         <v>1</v>
       </c>
@@ -9680,16 +9632,16 @@
       <c r="L27" s="34"/>
     </row>
     <row r="28" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A28" s="182" t="s">
+      <c r="A28" s="213" t="s">
         <v>348</v>
       </c>
-      <c r="B28" s="183"/>
-      <c r="C28" s="183"/>
-      <c r="D28" s="184"/>
-      <c r="E28" s="185"/>
-      <c r="F28" s="186"/>
-      <c r="G28" s="187"/>
-      <c r="H28" s="188"/>
+      <c r="B28" s="179"/>
+      <c r="C28" s="179"/>
+      <c r="D28" s="180"/>
+      <c r="E28" s="181"/>
+      <c r="F28" s="182"/>
+      <c r="G28" s="183"/>
+      <c r="H28" s="184"/>
       <c r="I28" s="37"/>
       <c r="J28" s="36">
         <f>J27+I28</f>
@@ -10018,10 +9970,10 @@
       <c r="L37" s="12"/>
     </row>
     <row r="38" spans="1:12" ht="21" customHeight="1">
-      <c r="A38" s="189"/>
-      <c r="B38" s="181"/>
-      <c r="C38" s="181"/>
-      <c r="D38" s="190"/>
+      <c r="A38" s="214"/>
+      <c r="B38" s="186"/>
+      <c r="C38" s="186"/>
+      <c r="D38" s="187"/>
       <c r="E38" s="12"/>
       <c r="F38" s="43"/>
       <c r="G38" s="44"/>
@@ -10032,37 +9984,37 @@
       <c r="L38" s="12"/>
     </row>
     <row r="39" spans="1:12" ht="114" customHeight="1">
-      <c r="A39" s="217" t="s">
+      <c r="A39" s="227" t="s">
         <v>351</v>
       </c>
-      <c r="B39" s="218"/>
-      <c r="C39" s="218"/>
-      <c r="D39" s="192"/>
-      <c r="E39" s="193"/>
-      <c r="F39" s="194"/>
-      <c r="G39" s="195"/>
-      <c r="H39" s="196"/>
+      <c r="B39" s="221"/>
+      <c r="C39" s="221"/>
+      <c r="D39" s="216"/>
+      <c r="E39" s="188"/>
+      <c r="F39" s="189"/>
+      <c r="G39" s="190"/>
+      <c r="H39" s="191"/>
       <c r="I39" s="39"/>
       <c r="J39" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K39" s="178"/>
+      <c r="K39" s="210"/>
       <c r="L39" s="12"/>
     </row>
     <row r="40" spans="1:12" ht="145.5" customHeight="1">
-      <c r="A40" s="219" t="s">
+      <c r="A40" s="228" t="s">
         <v>350</v>
       </c>
-      <c r="B40" s="218"/>
-      <c r="C40" s="218"/>
-      <c r="D40" s="190"/>
-      <c r="E40" s="193"/>
-      <c r="F40" s="194"/>
-      <c r="G40" s="195"/>
-      <c r="H40" s="196"/>
+      <c r="B40" s="221"/>
+      <c r="C40" s="221"/>
+      <c r="D40" s="187"/>
+      <c r="E40" s="188"/>
+      <c r="F40" s="189"/>
+      <c r="G40" s="190"/>
+      <c r="H40" s="191"/>
       <c r="I40" s="39"/>
       <c r="J40" s="52"/>
-      <c r="K40" s="179"/>
+      <c r="K40" s="211"/>
     </row>
     <row r="41" spans="1:12" ht="12.75" customHeight="1">
       <c r="A41" s="28"/>
@@ -10403,13 +10355,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:H7"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:H5"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="D39:H40"/>
     <mergeCell ref="K39:K40"/>
@@ -10419,6 +10364,13 @@
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="A28:H28"/>
     <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:H7"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:H5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10456,112 +10408,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="185" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="195"/>
-      <c r="H1" s="196"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="189"/>
+      <c r="G1" s="190"/>
+      <c r="H1" s="191"/>
     </row>
     <row r="2" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A2" s="223" t="s">
+      <c r="A2" s="220" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="225"/>
-      <c r="F2" s="224"/>
-      <c r="G2" s="226"/>
-      <c r="H2" s="227"/>
+      <c r="B2" s="221"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="224"/>
+      <c r="H2" s="225"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A3" s="228" t="s">
+      <c r="A3" s="226" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="218"/>
-      <c r="C3" s="218"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="225"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="226"/>
-      <c r="H3" s="227"/>
+      <c r="B3" s="221"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="222"/>
+      <c r="E3" s="223"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="224"/>
+      <c r="H3" s="225"/>
       <c r="I3" s="35"/>
       <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A4" s="220" t="s">
+      <c r="A4" s="217" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="222" t="s">
+      <c r="B4" s="219" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="221"/>
-      <c r="D4" s="221"/>
-      <c r="E4" s="221"/>
-      <c r="F4" s="221"/>
-      <c r="G4" s="221"/>
-      <c r="H4" s="221"/>
+      <c r="C4" s="218"/>
+      <c r="D4" s="218"/>
+      <c r="E4" s="218"/>
+      <c r="F4" s="218"/>
+      <c r="G4" s="218"/>
+      <c r="H4" s="218"/>
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A5" s="221"/>
-      <c r="B5" s="221"/>
-      <c r="C5" s="221"/>
-      <c r="D5" s="221"/>
-      <c r="E5" s="221"/>
-      <c r="F5" s="221"/>
-      <c r="G5" s="221"/>
-      <c r="H5" s="221"/>
+      <c r="A5" s="218"/>
+      <c r="B5" s="218"/>
+      <c r="C5" s="218"/>
+      <c r="D5" s="218"/>
+      <c r="E5" s="218"/>
+      <c r="F5" s="218"/>
+      <c r="G5" s="218"/>
+      <c r="H5" s="218"/>
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" hidden="1" customHeight="1">
-      <c r="A6" s="220" t="s">
+      <c r="A6" s="217" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="222" t="s">
+      <c r="B6" s="219" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="221"/>
-      <c r="D6" s="221"/>
-      <c r="E6" s="221"/>
-      <c r="F6" s="221"/>
-      <c r="G6" s="221"/>
-      <c r="H6" s="221"/>
+      <c r="C6" s="218"/>
+      <c r="D6" s="218"/>
+      <c r="E6" s="218"/>
+      <c r="F6" s="218"/>
+      <c r="G6" s="218"/>
+      <c r="H6" s="218"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:12" ht="10.5" hidden="1" customHeight="1">
-      <c r="A7" s="221"/>
-      <c r="B7" s="221"/>
-      <c r="C7" s="221"/>
-      <c r="D7" s="221"/>
-      <c r="E7" s="221"/>
-      <c r="F7" s="221"/>
-      <c r="G7" s="221"/>
-      <c r="H7" s="221"/>
+      <c r="A7" s="218"/>
+      <c r="B7" s="218"/>
+      <c r="C7" s="218"/>
+      <c r="D7" s="218"/>
+      <c r="E7" s="218"/>
+      <c r="F7" s="218"/>
+      <c r="G7" s="218"/>
+      <c r="H7" s="218"/>
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A8" s="197" t="s">
+      <c r="A8" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="183"/>
-      <c r="C8" s="183"/>
-      <c r="D8" s="184"/>
-      <c r="E8" s="185"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="187"/>
-      <c r="H8" s="188"/>
+      <c r="B8" s="179"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="183"/>
+      <c r="H8" s="184"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
     </row>
@@ -10926,16 +10878,16 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A20" s="182" t="s">
+      <c r="A20" s="213" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="183"/>
-      <c r="C20" s="183"/>
-      <c r="D20" s="184"/>
-      <c r="E20" s="185"/>
-      <c r="F20" s="186"/>
-      <c r="G20" s="187"/>
-      <c r="H20" s="188"/>
+      <c r="B20" s="179"/>
+      <c r="C20" s="179"/>
+      <c r="D20" s="180"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="183"/>
+      <c r="H20" s="184"/>
       <c r="I20" s="37">
         <v>0</v>
       </c>
@@ -11079,16 +11031,16 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A25" s="182" t="s">
+      <c r="A25" s="213" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="183"/>
-      <c r="C25" s="183"/>
-      <c r="D25" s="184"/>
-      <c r="E25" s="185"/>
-      <c r="F25" s="186"/>
-      <c r="G25" s="187"/>
-      <c r="H25" s="188"/>
+      <c r="B25" s="179"/>
+      <c r="C25" s="179"/>
+      <c r="D25" s="180"/>
+      <c r="E25" s="181"/>
+      <c r="F25" s="182"/>
+      <c r="G25" s="183"/>
+      <c r="H25" s="184"/>
       <c r="I25" s="37">
         <v>1</v>
       </c>
@@ -11244,16 +11196,16 @@
       <c r="L29" s="34"/>
     </row>
     <row r="30" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A30" s="182" t="s">
+      <c r="A30" s="213" t="s">
         <v>348</v>
       </c>
-      <c r="B30" s="183"/>
-      <c r="C30" s="183"/>
-      <c r="D30" s="184"/>
-      <c r="E30" s="185"/>
-      <c r="F30" s="186"/>
-      <c r="G30" s="187"/>
-      <c r="H30" s="188"/>
+      <c r="B30" s="179"/>
+      <c r="C30" s="179"/>
+      <c r="D30" s="180"/>
+      <c r="E30" s="181"/>
+      <c r="F30" s="182"/>
+      <c r="G30" s="183"/>
+      <c r="H30" s="184"/>
       <c r="I30" s="37"/>
       <c r="J30" s="36">
         <f>J29+I30</f>
@@ -11619,10 +11571,10 @@
       <c r="L40" s="12"/>
     </row>
     <row r="41" spans="1:12" ht="21" customHeight="1">
-      <c r="A41" s="189"/>
-      <c r="B41" s="181"/>
-      <c r="C41" s="181"/>
-      <c r="D41" s="190"/>
+      <c r="A41" s="214"/>
+      <c r="B41" s="186"/>
+      <c r="C41" s="186"/>
+      <c r="D41" s="187"/>
       <c r="E41" s="12"/>
       <c r="F41" s="43"/>
       <c r="G41" s="44"/>
@@ -11633,37 +11585,37 @@
       <c r="L41" s="12"/>
     </row>
     <row r="42" spans="1:12" ht="114" customHeight="1">
-      <c r="A42" s="217" t="s">
+      <c r="A42" s="227" t="s">
         <v>351</v>
       </c>
-      <c r="B42" s="218"/>
-      <c r="C42" s="218"/>
-      <c r="D42" s="192"/>
-      <c r="E42" s="193"/>
-      <c r="F42" s="194"/>
-      <c r="G42" s="195"/>
-      <c r="H42" s="196"/>
+      <c r="B42" s="221"/>
+      <c r="C42" s="221"/>
+      <c r="D42" s="216"/>
+      <c r="E42" s="188"/>
+      <c r="F42" s="189"/>
+      <c r="G42" s="190"/>
+      <c r="H42" s="191"/>
       <c r="I42" s="39"/>
       <c r="J42" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K42" s="178"/>
+      <c r="K42" s="210"/>
       <c r="L42" s="12"/>
     </row>
     <row r="43" spans="1:12" ht="145.5" customHeight="1">
-      <c r="A43" s="219" t="s">
+      <c r="A43" s="228" t="s">
         <v>350</v>
       </c>
-      <c r="B43" s="218"/>
-      <c r="C43" s="218"/>
-      <c r="D43" s="190"/>
-      <c r="E43" s="193"/>
-      <c r="F43" s="194"/>
-      <c r="G43" s="195"/>
-      <c r="H43" s="196"/>
+      <c r="B43" s="221"/>
+      <c r="C43" s="221"/>
+      <c r="D43" s="187"/>
+      <c r="E43" s="188"/>
+      <c r="F43" s="189"/>
+      <c r="G43" s="190"/>
+      <c r="H43" s="191"/>
       <c r="I43" s="39"/>
       <c r="J43" s="52"/>
-      <c r="K43" s="179"/>
+      <c r="K43" s="211"/>
     </row>
     <row r="44" spans="1:12" ht="12.75" customHeight="1">
       <c r="A44" s="28"/>

</xml_diff>